<commit_message>
Testplan Updated , new testcase updated
</commit_message>
<xml_diff>
--- a/Docs/TestPlan of Serdes Final.xlsx
+++ b/Docs/TestPlan of Serdes Final.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Test Plan" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="ASSERTION" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="Coverage" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="4" state="hidden" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -166,7 +166,17 @@
     <t xml:space="preserve">cp_tx_expected</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Zero = {0};       2. Non Zero = {[1:1023]};</t>
+    <t xml:space="preserve">1. Zero = {0};       
+2. Walking One = {1,2,4,8,16,32,64,128,256,512}; 
+3. Walking Zero = {1022, 1021, 1019, 1015, 1007, 991, 959, 895, 767, 511};
+4. ALTERNATE_5 = {341};
+5. ALTERNATE_A = {682};
+6. All_One = {1023};
+7. Increment = {[1:100]};
+8. Low_range = {[1:255]};
+9. mid_range = {[256:511]};             
+10.high_range = {[512:767]};             
+11. max_range = {[768:1023]};</t>
   </si>
   <si>
     <t xml:space="preserve">cp_tx_actual</t>
@@ -271,18 +281,17 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="28"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="0"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -334,80 +343,92 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -420,23 +441,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
@@ -619,253 +623,253 @@
   </sheetPr>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="82.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="21.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="20.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="22.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="114.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="10.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="39.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="82.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="21.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="20.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="22.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="114.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="15.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="10.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="4" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+    <row r="2" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="n">
+      <c r="A3" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="7" t="s">
+      <c r="E3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="45.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="n">
+      <c r="A4" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="7" t="s">
+      <c r="E4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="66.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
+      <c r="A5" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="7" t="s">
+      <c r="E5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="58.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="n">
+      <c r="A6" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="7" t="s">
+      <c r="F6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="n">
+      <c r="A7" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="7" t="s">
+      <c r="F7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="50.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="n">
+      <c r="A8" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="7" t="s">
+      <c r="F8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="64.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="n">
+      <c r="A9" s="8" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="2"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="2"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="3"/>
-      <c r="D12" s="0"/>
-      <c r="E12" s="0"/>
-      <c r="F12" s="0"/>
-      <c r="G12" s="0"/>
+      <c r="B12" s="4"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="3"/>
-      <c r="D13" s="0"/>
-      <c r="E13" s="0"/>
-      <c r="F13" s="0"/>
-      <c r="G13" s="0"/>
+      <c r="B13" s="4"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="3"/>
-      <c r="D14" s="0"/>
-      <c r="E14" s="0"/>
-      <c r="F14" s="0"/>
-      <c r="G14" s="0"/>
+      <c r="B14" s="4"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="0"/>
-      <c r="E15" s="0"/>
-      <c r="F15" s="0"/>
-      <c r="G15" s="0"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -885,105 +889,105 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="11" width="83.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="15.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="12" width="83.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="15.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="4" t="s">
+      <c r="A1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+    <row r="2" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="35.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="n">
+      <c r="A3" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="35.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="n">
+      <c r="A4" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="35.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
+      <c r="A5" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="n">
+      <c r="A6" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="35.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="n">
+      <c r="A7" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1005,86 +1009,86 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="46.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="77.09"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="89.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="14" t="s">
+    <row r="1" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" customFormat="false" ht="65.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" s="16" customFormat="true" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="6" t="s">
         <v>43</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="35.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="n">
+    <row r="3" customFormat="false" ht="215.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="18" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="35.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="n">
+    <row r="4" customFormat="false" ht="229.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="13" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="35.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="n">
+    <row r="5" customFormat="false" ht="260.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="13" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="35.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="n">
+    <row r="6" customFormat="false" ht="224.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="13" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="19" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1109,69 +1113,69 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="195.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="464.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="20"/>
+      <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="195.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>